<commit_message>
Added Test Case and Test Data for VLink AuthCapture.
</commit_message>
<xml_diff>
--- a/KatalonData/VLinkSmokeData.xlsx
+++ b/KatalonData/VLinkSmokeData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{EE89E0B6-2EF8-485E-AB49-15CBEF5801DC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{56FBFC1A-DB4D-4179-B902-135381CD1D51}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView windowHeight="17640" windowWidth="29040" xWindow="-120" xr2:uid="{D3A86137-2393-48B3-A2A1-24E657E7CF34}" yWindow="-120"/>
+    <workbookView activeTab="1" windowHeight="14730" windowWidth="16665" xWindow="7950" xr2:uid="{D3A86137-2393-48B3-A2A1-24E657E7CF34}" yWindow="2670"/>
   </bookViews>
   <sheets>
     <sheet name="Auth" r:id="rId1" sheetId="1"/>
+    <sheet name="AuthCapture" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="59">
   <si>
     <t>Result</t>
   </si>
@@ -134,21 +135,6 @@
     <t>5146312200000035</t>
   </si>
   <si>
-    <t>Mon Oct 03 22:15:00 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Oct 03 22:15:19 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Oct 03 22:15:36 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Oct 03 22:15:52 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Oct 03 22:16:10 EDT 2022</t>
-  </si>
-  <si>
     <t>health</t>
   </si>
   <si>
@@ -158,22 +144,76 @@
     <t>pwd3136</t>
   </si>
   <si>
+    <t>Mon Oct 03 22:22:36 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Oct 03 22:22:51 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Oct 03 22:23:06 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Oct 03 22:23:20 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Oct 03 22:23:35 EDT 2022</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Mon Oct 03 22:22:36 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Oct 03 22:22:51 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Oct 03 22:23:06 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Oct 03 22:23:20 EDT 2022</t>
-  </si>
-  <si>
-    <t>Mon Oct 03 22:23:35 EDT 2022</t>
+    <t>Tue Oct 04 20:55:15 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 04 20:55:42 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 04 20:56:08 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 04 20:56:33 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 04 20:57:01 EDT 2022</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Tue Oct 04 20:59:12 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 04 20:59:27 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 04 20:59:40 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 04 20:59:53 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 04 21:00:06 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 04 21:02:26 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 04 21:02:41 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 04 21:04:53 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 04 21:05:17 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 04 21:05:40 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 04 21:06:02 EDT 2022</t>
+  </si>
+  <si>
+    <t>Tue Oct 04 21:06:25 EDT 2022</t>
   </si>
 </sst>
 </file>
@@ -556,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B3BF19-5985-4984-B3CC-B3E33E12951F}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,7 +670,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -677,7 +717,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -724,7 +764,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -771,7 +811,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -792,7 +832,7 @@
         <v>2435</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="J5" s="2">
         <v>11111111</v>
@@ -818,7 +858,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -839,10 +879,10 @@
         <v>3136</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>17</v>
@@ -864,4 +904,317 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77641590-759F-4E9F-886E-0EE016894C97}">
+  <dimension ref="A1:P6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="27.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="15.42578125" collapsed="true"/>
+    <col min="4" max="4" style="2" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="2" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="2" width="13.28515625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="2" width="12.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="2" width="18.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="2" width="15.5703125" collapsed="true"/>
+    <col min="11" max="11" style="2" width="9.140625" collapsed="true"/>
+    <col min="12" max="12" style="1" width="9.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="23.7109375" collapsed="true"/>
+    <col min="14" max="16384" style="2" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2">
+        <v>234</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="2">
+        <v>12</v>
+      </c>
+      <c r="O2" s="2">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2">
+        <v>234</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="2">
+        <v>12</v>
+      </c>
+      <c r="O3" s="2">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2">
+        <v>234</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="2">
+        <v>12</v>
+      </c>
+      <c r="O4" s="2">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2">
+        <v>87</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2435</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="2">
+        <v>11111111</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="2">
+        <v>12</v>
+      </c>
+      <c r="O5" s="2">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2">
+        <v>581</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="2">
+        <v>3136</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N6" s="2">
+        <v>12</v>
+      </c>
+      <c r="O6" s="2">
+        <v>2029</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Test Case and Data for VRelayLiveApps in Upgrade.
</commit_message>
<xml_diff>
--- a/KatalonData/VLinkSmokeData.xlsx
+++ b/KatalonData/VLinkSmokeData.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="84">
   <si>
     <t>Result</t>
   </si>
@@ -259,6 +259,36 @@
   </si>
   <si>
     <t>Fri Oct 21 13:54:23 EDT 2022</t>
+  </si>
+  <si>
+    <t>Thu Oct 27 10:04:04 EDT 2022</t>
+  </si>
+  <si>
+    <t>Thu Oct 27 10:04:27 EDT 2022</t>
+  </si>
+  <si>
+    <t>Thu Oct 27 10:04:43 EDT 2022</t>
+  </si>
+  <si>
+    <t>Thu Oct 27 10:05:01 EDT 2022</t>
+  </si>
+  <si>
+    <t>Thu Oct 27 10:05:17 EDT 2022</t>
+  </si>
+  <si>
+    <t>Thu Oct 27 10:05:34 EDT 2022</t>
+  </si>
+  <si>
+    <t>Thu Oct 27 10:05:59 EDT 2022</t>
+  </si>
+  <si>
+    <t>Thu Oct 27 10:06:23 EDT 2022</t>
+  </si>
+  <si>
+    <t>Thu Oct 27 10:06:47 EDT 2022</t>
+  </si>
+  <si>
+    <t>Thu Oct 27 10:07:11 EDT 2022</t>
   </si>
 </sst>
 </file>
@@ -715,7 +745,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -762,7 +792,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -809,7 +839,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -856,7 +886,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -903,7 +933,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -1029,7 +1059,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -1076,7 +1106,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -1123,7 +1153,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -1170,7 +1200,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -1217,7 +1247,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Executed TestMinusAndAtSigns Test case.
</commit_message>
<xml_diff>
--- a/KatalonData/VLinkSmokeData.xlsx
+++ b/KatalonData/VLinkSmokeData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AE9E3B-EC7B-452F-9634-E48B5F4D3018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66827845-26D4-47DD-8B0B-0DA457B5316F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{D3A86137-2393-48B3-A2A1-24E657E7CF34}"/>
   </bookViews>
@@ -10447,7 +10447,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated VLink Smoke Test Cases.
</commit_message>
<xml_diff>
--- a/KatalonData/VLinkSmokeData.xlsx
+++ b/KatalonData/VLinkSmokeData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{FCDE6067-6DD8-4454-840D-79F3834ACE5A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{D96B97DE-22D2-49C7-B2EE-7B13F16F07D1}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="19" firstSheet="11" windowHeight="17640" windowWidth="29040" xWindow="-120" xr2:uid="{D3A86137-2393-48B3-A2A1-24E657E7CF34}" yWindow="-120"/>
+    <workbookView activeTab="7" firstSheet="1" tabRatio="887" windowHeight="14565" windowWidth="18810" xWindow="4410" xr2:uid="{D3A86137-2393-48B3-A2A1-24E657E7CF34}" yWindow="1665"/>
   </bookViews>
   <sheets>
     <sheet name="Auth" r:id="rId1" sheetId="1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3062" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3074" uniqueCount="299">
   <si>
     <t>Result</t>
   </si>
@@ -780,9 +780,6 @@
     <t>Tue Apr 25 14:04:42 EDT 2023</t>
   </si>
   <si>
-    <t>Tue Apr 25 14:04:56 EDT 2023</t>
-  </si>
-  <si>
     <t>Tue Apr 25 14:05:10 EDT 2023</t>
   </si>
   <si>
@@ -795,9 +792,6 @@
     <t>Tue Apr 25 14:06:18 EDT 2023</t>
   </si>
   <si>
-    <t>Tue Apr 25 14:06:43 EDT 2023</t>
-  </si>
-  <si>
     <t>Tue Apr 25 14:07:07 EDT 2023</t>
   </si>
   <si>
@@ -810,9 +804,6 @@
     <t>Tue Apr 25 14:08:24 EDT 2023</t>
   </si>
   <si>
-    <t>Tue Apr 25 14:08:52 EDT 2023</t>
-  </si>
-  <si>
     <t>Tue Apr 25 14:10:00 EDT 2023</t>
   </si>
   <si>
@@ -840,9 +831,6 @@
     <t>Tue Apr 25 14:12:11 EDT 2023</t>
   </si>
   <si>
-    <t>Tue Apr 25 14:12:35 EDT 2023</t>
-  </si>
-  <si>
     <t>Tue Apr 25 14:12:59 EDT 2023</t>
   </si>
   <si>
@@ -897,15 +885,6 @@
     <t>Tue Apr 25 14:21:59 EDT 2023</t>
   </si>
   <si>
-    <t>Tue Apr 25 14:52:11 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Apr 25 14:52:26 EDT 2023</t>
-  </si>
-  <si>
-    <t>Tue Apr 25 14:52:42 EDT 2023</t>
-  </si>
-  <si>
     <t>Vantiv CPS Dual CF</t>
   </si>
   <si>
@@ -933,10 +912,46 @@
     <t>dsfsdf46346543</t>
   </si>
   <si>
+    <t>Wed Jul 12 09:51:58 EDT 2023</t>
+  </si>
+  <si>
+    <t>4761739001010135</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 15:13:50 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 15:14:09 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 15:22:59 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 15:29:10 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 15:33:49 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 15:34:07 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 15:34:22 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 15:37:04 EST 2023</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Wed Jul 12 09:51:58 EDT 2023</t>
+    <t>Tue Dec 12 15:42:47 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 15:43:03 EST 2023</t>
+  </si>
+  <si>
+    <t>Tue Dec 12 15:43:18 EST 2023</t>
   </si>
 </sst>
 </file>
@@ -1711,7 +1726,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -1758,7 +1773,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -1805,7 +1820,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -1852,7 +1867,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -1899,7 +1914,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -2024,7 +2039,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -2071,7 +2086,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -2118,7 +2133,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -2165,7 +2180,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -2212,7 +2227,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -2339,7 +2354,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>296</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -2386,7 +2401,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>21</v>
@@ -2433,7 +2448,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>279</v>
+        <v>298</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>22</v>
@@ -10475,7 +10490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79DCF843-7CC4-48A5-8072-F1A801B90CE0}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -10485,15 +10500,14 @@
     <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="27.140625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" style="2" width="15.42578125" collapsed="true"/>
     <col min="4" max="4" style="2" width="9.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="21.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="2" width="21.0" collapsed="true"/>
     <col min="6" max="6" customWidth="true" style="2" width="12.140625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" style="2" width="14.140625" collapsed="true"/>
     <col min="8" max="8" customWidth="true" style="2" width="13.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="2" width="21.42578125" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" style="2" width="21.42578125" collapsed="true"/>
     <col min="10" max="10" style="2" width="9.140625" collapsed="true"/>
     <col min="11" max="11" style="1" width="9.140625" collapsed="true"/>
-    <col min="12" max="17" style="2" width="9.140625" collapsed="false"/>
-    <col min="18" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="12" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -10510,7 +10524,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>111</v>
@@ -10536,13 +10550,13 @@
         <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="F2" s="2">
         <v>234</v>
@@ -10572,8 +10586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F862F746-9284-4D5F-8449-DC04488EA2C6}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10646,7 +10660,7 @@
         <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -10693,7 +10707,7 @@
         <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -10834,7 +10848,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>241</v>
+        <v>287</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -10877,8 +10891,14 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>288</v>
+      </c>
       <c r="C7" s="2" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>25</v>
@@ -10887,19 +10907,19 @@
         <v>591</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="H7" s="2">
         <v>4494</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>17</v>
@@ -10908,7 +10928,7 @@
         <v>10.5</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>31</v>
+        <v>286</v>
       </c>
       <c r="N7" s="2">
         <v>12</v>
@@ -10927,7 +10947,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11000,7 +11020,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -11047,7 +11067,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -11094,7 +11114,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -11141,7 +11161,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -11185,10 +11205,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>246</v>
+        <v>289</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -11221,7 +11241,7 @@
         <v>10.5</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>31</v>
+        <v>286</v>
       </c>
       <c r="N6" s="2">
         <v>12</v>
@@ -11240,7 +11260,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11313,7 +11333,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -11360,7 +11380,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -11407,7 +11427,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -11454,7 +11474,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -11501,7 +11521,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>251</v>
+        <v>290</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -11552,7 +11572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C85066F-A70F-4EC6-96A2-3B11D71E8332}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
@@ -11620,7 +11640,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -11661,7 +11681,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>21</v>
@@ -11702,7 +11722,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>22</v>
@@ -11821,7 +11841,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -11868,7 +11888,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -11915,7 +11935,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -11962,7 +11982,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -12009,7 +12029,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -12060,8 +12080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407A61CA-7BCD-4622-83EC-6EE78F45F1F1}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12134,7 +12154,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -12181,7 +12201,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -12228,7 +12248,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -12275,7 +12295,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -12319,10 +12339,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>261</v>
+        <v>294</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -12447,7 +12467,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -12494,7 +12514,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -12541,7 +12561,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -12588,7 +12608,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -12635,7 +12655,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Updated Upgrade and Production Live Processors test cases with Visa Debit Cards
</commit_message>
<xml_diff>
--- a/KatalonData/VLinkSmokeData.xlsx
+++ b/KatalonData/VLinkSmokeData.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3926" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5026" uniqueCount="787">
   <si>
     <t>Result</t>
   </si>
@@ -1591,6 +1591,831 @@
   </si>
   <si>
     <t>Mon May 27 19:23:02 EDT 2024</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 22:42:52 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 22:45:08 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 22:47:23 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 22:49:36 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 22:49:40 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 22:50:01 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 22:52:16 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 22:56:42 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:01:06 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:01:12 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:01:15 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:03:27 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:05:41 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:07:56 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:08:00 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:08:03 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:08:17 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:12:44 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:17:13 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:21:41 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:21:44 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:21:48 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:26:15 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:28:30 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:32:57 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:33:00 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:33:03 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:35:14 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:35:19 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:35:21 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:35:26 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:35:29 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:35:31 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:35:33 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:35:35 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:39:58 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:44:25 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:48:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:48:54 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:48:59 EDT 2025</t>
+  </si>
+  <si>
+    <t>Wed Aug 20 23:55:43 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:02:22 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:06:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:06:55 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:06:58 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:13:36 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:15:49 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:20:15 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:20:19 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:20:22 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:27:01 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:31:27 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:33:42 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:33:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:33:49 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:33:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:33:56 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:33:59 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:34:09 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:34:18 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:34:27 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:34:36 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:34:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:34:55 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:35:04 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:35:13 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:35:22 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:35:32 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:35:41 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:35:50 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:35:59 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:36:09 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:36:18 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:36:27 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:36:36 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:36:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:36:55 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:37:05 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:37:15 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:37:24 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:37:34 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:37:43 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:37:52 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:38:02 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:38:11 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:38:20 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:38:29 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:38:39 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:38:48 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:38:57 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:00 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:03 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:07 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:10 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:13 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:17 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:20 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:23 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:26 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:29 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:33 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:36 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:39 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:43 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:46 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:49 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:53 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:56 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:39:59 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:02 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:06 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:09 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:12 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:16 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:19 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:22 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:25 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:28 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:32 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:35 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:38 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:41 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:44 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:46 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:48 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:53 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:55 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:40:57 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:41:00 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:41:02 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:41:05 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:41:08 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:41:10 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:41:13 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:41:15 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:41:17 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:41:20 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:41:23 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:41:25 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:41:27 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:41:30 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:41:32 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 00:41:35 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 03:34:00 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 03:34:03 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 03:34:06 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 03:34:09 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 03:34:11 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 03:34:14 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 12:50:00 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:23:16 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:23:21 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:23:24 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:23:29 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:23:35 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:23:39 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:23:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:23:48 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:23:54 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:24:00 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:24:05 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:24:09 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:24:12 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:24:15 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:24:20 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:24:24 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:24:28 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:24:32 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:24:37 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:24:43 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:24:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:24:54 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:25:01 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:25:08 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:25:13 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:25:18 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:25:24 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:25:27 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:25:30 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:25:34 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:25:36 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:25:39 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:25:41 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:25:44 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:25:47 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:26:53 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:27:21 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:27:49 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:28:37 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:28:43 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:28:48 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:28:50 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:28:58 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:29:16 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:29:19 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:29:26 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:29:32 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:29:39 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:30:12 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:30:32 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:30:35 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:30:37 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:30:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:30:47 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:30:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:30:54 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 21 22:31:11 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:26:49 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:26:56 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:27:00 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:27:06 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:27:12 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:29:43 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:29:53 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:30:03 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:30:17 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:30:27 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:51:57 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:52:05 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:52:12 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:52:19 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:52:26 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:52:34 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:52:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:52:55 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:53:06 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:53:19 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:53:29 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:53:36 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:53:42 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:53:49 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:53:57 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:54:05 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:54:13 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:54:24 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:54:34 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:54:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:54:55 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:55:06 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:55:18 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:55:30 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:55:41 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:55:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:56:03 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:56:10 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:56:16 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:56:23 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:56:29 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:56:36 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:56:42 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:56:49 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:56:55 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:57:06 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:57:17 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:57:27 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:57:39 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:57:49 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:58:05 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:58:19 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:58:39 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:58:53 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:59:08 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:59:26 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 17:59:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 18:00:00 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 18:00:15 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 18:00:31 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 18:00:46 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 18:01:00 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 18:01:14 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 18:01:29 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 18:01:43 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 18:01:47 EDT 2025</t>
+  </si>
+  <si>
+    <t>Fri Aug 22 18:01:53 EDT 2025</t>
   </si>
 </sst>
 </file>
@@ -2048,7 +2873,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>455</v>
+        <v>730</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -2095,7 +2920,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>456</v>
+        <v>731</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -2142,7 +2967,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>457</v>
+        <v>732</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -2189,7 +3014,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>458</v>
+        <v>733</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -2236,7 +3061,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>459</v>
+        <v>734</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -2365,7 +3190,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>499</v>
+        <v>774</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -2412,7 +3237,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>500</v>
+        <v>775</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -2459,7 +3284,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>501</v>
+        <v>776</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -2506,7 +3331,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>502</v>
+        <v>777</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -2553,7 +3378,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>503</v>
+        <v>778</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -2678,7 +3503,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>504</v>
+        <v>779</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -2725,7 +3550,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>505</v>
+        <v>780</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -2772,7 +3597,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>506</v>
+        <v>781</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -2819,7 +3644,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>507</v>
+        <v>782</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -2866,7 +3691,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>508</v>
+        <v>783</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -2993,7 +3818,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>509</v>
+        <v>784</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -3040,7 +3865,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>510</v>
+        <v>785</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>21</v>
@@ -3087,7 +3912,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>511</v>
+        <v>786</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>22</v>
@@ -3321,7 +4146,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>356</v>
+        <v>569</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>20</v>
@@ -3441,7 +4266,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>357</v>
+        <v>570</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>20</v>
@@ -3561,7 +4386,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>358</v>
+        <v>571</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>20</v>
@@ -3681,7 +4506,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>359</v>
+        <v>572</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>20</v>
@@ -3801,7 +4626,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>360</v>
+        <v>573</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>20</v>
@@ -3921,7 +4746,7 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>361</v>
+        <v>574</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>20</v>
@@ -4041,7 +4866,7 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>362</v>
+        <v>575</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>20</v>
@@ -4162,7 +4987,7 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>363</v>
+        <v>576</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>20</v>
@@ -4283,7 +5108,7 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>364</v>
+        <v>577</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>20</v>
@@ -4404,7 +5229,7 @@
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>365</v>
+        <v>578</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>20</v>
@@ -4524,7 +5349,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>366</v>
+        <v>579</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>20</v>
@@ -4644,7 +5469,7 @@
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>367</v>
+        <v>580</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>20</v>
@@ -4764,7 +5589,7 @@
         <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>368</v>
+        <v>581</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>20</v>
@@ -4884,7 +5709,7 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>369</v>
+        <v>582</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>20</v>
@@ -5004,7 +5829,7 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>370</v>
+        <v>583</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>20</v>
@@ -5124,7 +5949,7 @@
         <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>371</v>
+        <v>584</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>20</v>
@@ -5244,7 +6069,7 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>372</v>
+        <v>585</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>20</v>
@@ -5364,7 +6189,7 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>373</v>
+        <v>586</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>20</v>
@@ -5484,7 +6309,7 @@
         <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>374</v>
+        <v>587</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>20</v>
@@ -5604,7 +6429,7 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>375</v>
+        <v>588</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>20</v>
@@ -5724,7 +6549,7 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>376</v>
+        <v>589</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>20</v>
@@ -5844,7 +6669,7 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>377</v>
+        <v>590</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>20</v>
@@ -5964,7 +6789,7 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>378</v>
+        <v>591</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>20</v>
@@ -6084,7 +6909,7 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>379</v>
+        <v>592</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>20</v>
@@ -6204,7 +7029,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>380</v>
+        <v>593</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>20</v>
@@ -6324,7 +7149,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>381</v>
+        <v>594</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>20</v>
@@ -6444,7 +7269,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>382</v>
+        <v>595</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>20</v>
@@ -6564,7 +7389,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>383</v>
+        <v>596</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>20</v>
@@ -6684,7 +7509,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>384</v>
+        <v>597</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>20</v>
@@ -6804,7 +7629,7 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>385</v>
+        <v>598</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>20</v>
@@ -6924,7 +7749,7 @@
         <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>386</v>
+        <v>599</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>20</v>
@@ -7044,7 +7869,7 @@
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>387</v>
+        <v>600</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>20</v>
@@ -7267,7 +8092,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>388</v>
+        <v>601</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>20</v>
@@ -7332,7 +8157,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>389</v>
+        <v>602</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>20</v>
@@ -7397,7 +8222,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>390</v>
+        <v>603</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>20</v>
@@ -7462,7 +8287,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>391</v>
+        <v>604</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>20</v>
@@ -7527,7 +8352,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>392</v>
+        <v>605</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>20</v>
@@ -7592,7 +8417,7 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>393</v>
+        <v>606</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>20</v>
@@ -7657,7 +8482,7 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>394</v>
+        <v>607</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>20</v>
@@ -7723,7 +8548,7 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>395</v>
+        <v>608</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>20</v>
@@ -7789,7 +8614,7 @@
         <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>396</v>
+        <v>609</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>20</v>
@@ -7855,7 +8680,7 @@
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>397</v>
+        <v>610</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>20</v>
@@ -7920,7 +8745,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>398</v>
+        <v>611</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>20</v>
@@ -7985,7 +8810,7 @@
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>399</v>
+        <v>612</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>20</v>
@@ -8050,7 +8875,7 @@
         <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>400</v>
+        <v>613</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>20</v>
@@ -8115,7 +8940,7 @@
         <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>401</v>
+        <v>614</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>20</v>
@@ -8180,7 +9005,7 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>402</v>
+        <v>615</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>20</v>
@@ -8242,10 +9067,10 @@
     </row>
     <row customFormat="1" ht="30" r="17" s="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
-        <v>403</v>
+        <v>616</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>20</v>
@@ -8310,7 +9135,7 @@
         <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>404</v>
+        <v>617</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>20</v>
@@ -8375,7 +9200,7 @@
         <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>405</v>
+        <v>618</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>20</v>
@@ -8437,10 +9262,10 @@
     </row>
     <row customFormat="1" ht="30" r="20" s="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="B20" t="s">
-        <v>406</v>
+        <v>619</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>20</v>
@@ -8505,7 +9330,7 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>407</v>
+        <v>620</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>20</v>
@@ -8570,7 +9395,7 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>408</v>
+        <v>621</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>20</v>
@@ -8635,7 +9460,7 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>409</v>
+        <v>622</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>20</v>
@@ -8700,7 +9525,7 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>410</v>
+        <v>623</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>20</v>
@@ -8765,7 +9590,7 @@
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>411</v>
+        <v>624</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>20</v>
@@ -8830,7 +9655,7 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>412</v>
+        <v>625</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>20</v>
@@ -8895,7 +9720,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>413</v>
+        <v>626</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>20</v>
@@ -8960,7 +9785,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>414</v>
+        <v>627</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>20</v>
@@ -9025,7 +9850,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>415</v>
+        <v>628</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>20</v>
@@ -9090,7 +9915,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>416</v>
+        <v>629</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>20</v>
@@ -9155,7 +9980,7 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>417</v>
+        <v>630</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>20</v>
@@ -9220,7 +10045,7 @@
         <v>28</v>
       </c>
       <c r="B32" t="s">
-        <v>418</v>
+        <v>631</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>20</v>
@@ -9285,7 +10110,7 @@
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>419</v>
+        <v>632</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>20</v>
@@ -9420,10 +10245,10 @@
     </row>
     <row customFormat="1" ht="30" r="2" s="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>420</v>
+        <v>633</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>20</v>
@@ -9461,7 +10286,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>421</v>
+        <v>634</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>20</v>
@@ -9499,7 +10324,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>422</v>
+        <v>635</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>20</v>
@@ -9538,7 +10363,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>423</v>
+        <v>636</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>20</v>
@@ -9573,10 +10398,10 @@
     </row>
     <row customFormat="1" r="6" s="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>424</v>
+        <v>637</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>20</v>
@@ -9614,7 +10439,7 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>425</v>
+        <v>638</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>20</v>
@@ -9652,7 +10477,7 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>426</v>
+        <v>639</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>20</v>
@@ -9690,7 +10515,7 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>427</v>
+        <v>640</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>20</v>
@@ -9795,10 +10620,10 @@
     </row>
     <row customFormat="1" ht="30" r="2" s="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>428</v>
+        <v>641</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>20</v>
@@ -9830,10 +10655,10 @@
     </row>
     <row customFormat="1" ht="30" r="3" s="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>429</v>
+        <v>642</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>20</v>
@@ -9865,10 +10690,10 @@
     </row>
     <row customFormat="1" ht="30" r="4" s="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>430</v>
+        <v>643</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>20</v>
@@ -9904,7 +10729,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>431</v>
+        <v>644</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>20</v>
@@ -9939,7 +10764,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>432</v>
+        <v>645</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>20</v>
@@ -9971,10 +10796,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>433</v>
+        <v>646</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>20</v>
@@ -10009,7 +10834,7 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>434</v>
+        <v>647</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>20</v>
@@ -10114,10 +10939,10 @@
     </row>
     <row customFormat="1" ht="30" r="2" s="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>435</v>
+        <v>648</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>20</v>
@@ -10155,7 +10980,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>436</v>
+        <v>649</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>20</v>
@@ -10193,7 +11018,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>437</v>
+        <v>650</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>20</v>
@@ -10232,7 +11057,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>438</v>
+        <v>651</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>20</v>
@@ -10270,7 +11095,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>439</v>
+        <v>652</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>20</v>
@@ -10305,10 +11130,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
-        <v>440</v>
+        <v>653</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>20</v>
@@ -10346,7 +11171,7 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>441</v>
+        <v>654</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>20</v>
@@ -10384,7 +11209,7 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>442</v>
+        <v>655</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>20</v>
@@ -10503,7 +11328,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>446</v>
+        <v>659</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>129</v>
@@ -10541,7 +11366,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>447</v>
+        <v>660</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>129</v>
@@ -10579,7 +11404,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>448</v>
+        <v>661</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>129</v>
@@ -10692,10 +11517,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>443</v>
+        <v>656</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>129</v>
@@ -10733,7 +11558,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>444</v>
+        <v>657</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>129</v>
@@ -10771,7 +11596,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>445</v>
+        <v>658</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>129</v>
@@ -10887,7 +11712,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>460</v>
+        <v>735</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -10934,7 +11759,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>461</v>
+        <v>736</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -10981,7 +11806,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>462</v>
+        <v>737</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -11028,7 +11853,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>463</v>
+        <v>738</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -11075,7 +11900,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>464</v>
+        <v>739</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -11299,7 +12124,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>465</v>
+        <v>740</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -11346,7 +12171,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>466</v>
+        <v>741</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -11393,7 +12218,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>467</v>
+        <v>742</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -11440,7 +12265,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>468</v>
+        <v>743</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -11487,7 +12312,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>469</v>
+        <v>744</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -11534,7 +12359,7 @@
         <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>470</v>
+        <v>745</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>276</v>
@@ -11659,7 +12484,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>471</v>
+        <v>746</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -11706,7 +12531,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>472</v>
+        <v>747</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -11753,7 +12578,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>473</v>
+        <v>748</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -11800,7 +12625,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>474</v>
+        <v>749</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -11847,7 +12672,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>475</v>
+        <v>750</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -11972,7 +12797,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>476</v>
+        <v>751</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -12019,7 +12844,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>477</v>
+        <v>752</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -12066,7 +12891,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>478</v>
+        <v>753</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -12113,7 +12938,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>479</v>
+        <v>754</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -12160,7 +12985,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>480</v>
+        <v>755</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -12279,7 +13104,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>481</v>
+        <v>756</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -12320,7 +13145,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>482</v>
+        <v>757</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>21</v>
@@ -12361,7 +13186,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>483</v>
+        <v>758</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>22</v>
@@ -12480,7 +13305,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>484</v>
+        <v>759</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -12527,7 +13352,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>485</v>
+        <v>760</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -12574,7 +13399,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>486</v>
+        <v>761</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -12621,7 +13446,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>487</v>
+        <v>762</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -12668,7 +13493,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>488</v>
+        <v>763</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -12793,7 +13618,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>489</v>
+        <v>764</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -12840,7 +13665,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>490</v>
+        <v>765</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -12887,7 +13712,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>491</v>
+        <v>766</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -12934,7 +13759,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>492</v>
+        <v>767</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -12981,7 +13806,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>493</v>
+        <v>768</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>
@@ -13106,7 +13931,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>494</v>
+        <v>769</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>20</v>
@@ -13153,7 +13978,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>495</v>
+        <v>770</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>20</v>
@@ -13200,7 +14025,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>496</v>
+        <v>771</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>20</v>
@@ -13247,7 +14072,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>497</v>
+        <v>772</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>21</v>
@@ -13294,7 +14119,7 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>498</v>
+        <v>773</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>22</v>

</xml_diff>